<commit_message>
Assemble the Dispatcher template
</commit_message>
<xml_diff>
--- a/Dispatcher/Config.xlsx
+++ b/Dispatcher/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="10703"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="10703" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Exception</t>
   </si>
   <si>
-    <t>Testing ReFrameWork</t>
-  </si>
-  <si>
     <t>love@uipath.com</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>Input queue for Performer template</t>
   </si>
   <si>
-    <t>Input data folder to OnloadQueue</t>
-  </si>
-  <si>
     <t>OffloadQueue: Queue to fetch data from</t>
   </si>
   <si>
@@ -255,6 +249,39 @@
   </si>
   <si>
     <t>OrchestratorLogin</t>
+  </si>
+  <si>
+    <t>Data folder from DownloadAttachments to OnloadQueue</t>
+  </si>
+  <si>
+    <t>EmailFilter</t>
+  </si>
+  <si>
+    <t>InboxFolder</t>
+  </si>
+  <si>
+    <t>Inbox</t>
+  </si>
+  <si>
+    <t>Filter criteria for incoming messages to DownloadAttachments</t>
+  </si>
+  <si>
+    <t>Mailbox folder to scan for messages for DownloadAttachments</t>
+  </si>
+  <si>
+    <t>@SQL="urn:schemas:httpmail:subject" like '%RFW%'</t>
+  </si>
+  <si>
+    <t>CompleteFolder</t>
+  </si>
+  <si>
+    <t>OffloadQueue: Folder where to park files after completion</t>
+  </si>
+  <si>
+    <t>Test ReFrameWork</t>
+  </si>
+  <si>
+    <t>../TestData/Processed</t>
   </si>
 </sst>
 </file>
@@ -307,11 +334,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -653,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -680,10 +708,10 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -694,7 +722,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -718,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -743,7 +771,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -751,10 +779,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -765,7 +793,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -784,7 +812,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -795,7 +823,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -833,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -872,13 +900,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -889,10 +917,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -918,10 +946,10 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -937,151 +965,184 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
+        <v>78</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="B12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>66</v>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
+      <c r="B18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId1"/>
+    <hyperlink ref="B22" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>